<commit_message>
handle bams with no header, update to assay template
</commit_message>
<xml_diff>
--- a/assay_data/ARAP_assays.xlsx
+++ b/assay_data/ARAP_assays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="3400" windowWidth="42580" windowHeight="26140" tabRatio="500"/>
+    <workbookView xWindow="5500" yWindow="2980" windowWidth="42580" windowHeight="26140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All_Assays" sheetId="1" r:id="rId1"/>
@@ -3091,7 +3091,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="486">
+  <cellStyleXfs count="489">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3143,6 +3143,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3672,7 +3675,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="486">
+  <cellStyles count="489">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4137,6 +4140,9 @@
     <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -4492,8 +4498,8 @@
   </sheetPr>
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D275" sqref="D275"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4675,6 +4681,12 @@
       <c r="P4" t="s">
         <v>869</v>
       </c>
+      <c r="AB4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC4" s="36" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:30">
       <c r="A5" t="s">
@@ -4794,12 +4806,6 @@
       </c>
       <c r="P10" t="s">
         <v>508</v>
-      </c>
-      <c r="AB10" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC10" s="36" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -10828,14 +10834,14 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C203:C213 C116:C201 C218:C280 C3:C111">
-      <formula1>$AC$1:$AC$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B203:B213 B116:B201 B218:B280 B4:B111">
-      <formula1>$AB$1:$AB$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B203:B213 B4:B111 B218:B280 B116:B201">
+      <formula1>$AB$1:$AB$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>AB1:AB10</formula1>
+      <formula1>AB1:AB9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C203:C213 C3:C111 C218:C280 C116:C201">
+      <formula1>$AC$1:$AC$9</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -10856,7 +10862,7 @@
   <dimension ref="A1:AD150"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>